<commit_message>
4 Ras Screener scenarios and 4 Ras Surveys scenarios automation completed
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66799AF2-98EC-8341-889D-D97556A1D4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDAE67-DC76-9040-9753-852BE6540B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25700" yWindow="500" windowWidth="25480" windowHeight="28300" activeTab="2" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="341">
   <si>
     <t>Question</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>16 years</t>
-  </si>
-  <si>
-    <t>diego1@test.com</t>
   </si>
   <si>
     <t>Please log in. Email</t>
@@ -918,9 +915,6 @@
     <t>Have you ever been diagnosed with a kidney problem?Some examples include: minor issues with kidney shape, underdeveloped kidney, missing kidney, or swollen kidney</t>
   </si>
   <si>
-    <t>ScreenerScenario1@email.com</t>
-  </si>
-  <si>
     <t>You are almost done!</t>
   </si>
   <si>
@@ -930,12 +924,6 @@
   Please feel free to call at any time if you have any questions regarding this protocol and ask to speak with the RASopathies Study nurse. Our toll-free phone number is 1-800-518-8474 or 301-212-5250. Thank you for your willingness to consider joining our research effort.  We could not do vital studies like this without the help of dedicated patients and families.  </t>
   </si>
   <si>
-    <t>Screener1First</t>
-  </si>
-  <si>
-    <t>Screener1Last</t>
-  </si>
-  <si>
     <t xml:space="preserve">We know that RASopathies are a group of syndromes that have a genetic basis.  In order to help us determine eligibility for the RASopathies Study, we also need to know about any genetic testing that has been completed.  We will need a copy of any test results.  </t>
   </si>
   <si>
@@ -970,12 +958,6 @@
   </si>
   <si>
     <t>kilograms</t>
-  </si>
-  <si>
-    <t>We know that RASopathies are a group of syndromes that have a genetic basis.  In order to help us determine eligibility for the RASopathies Study, we also need to know about any genetic testing that has been completed.</t>
-  </si>
-  <si>
-    <t>To determine eligibility for this study, we need to collect information about medical diagnoses.  These questions ask about general medical conditions, cancer and any prior diagnosis of a RASopathy.</t>
   </si>
   <si>
     <t>You are almost done! 
@@ -1141,6 +1123,18 @@
   </si>
   <si>
     <t>Do you have any of the following issues with your ears?  Please select all that apply. Option 4</t>
+  </si>
+  <si>
+    <t>charmsras1@yahoo.com</t>
+  </si>
+  <si>
+    <t>ScreenerOneLast</t>
+  </si>
+  <si>
+    <t>ScreenerOneFirst</t>
+  </si>
+  <si>
+    <t>RASTest2022$$</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1565,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1601,7 +1595,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>273</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1617,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>274</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1718,7 +1712,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>270</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1726,7 +1720,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>270</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1777,9 +1771,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>288</v>
+        <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>38</v>
@@ -1809,12 +1803,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -1883,10 +1877,10 @@
     </row>
     <row r="39" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1902,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA38AB1-F752-BB4E-9CFB-C6D8167B319F}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1923,18 +1917,18 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="4">
-        <v>123456</v>
+        <v>96</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
@@ -1950,7 +1944,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -1958,12 +1952,12 @@
         <v>60</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -1971,7 +1965,7 @@
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
@@ -2019,7 +2013,7 @@
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>15</v>
@@ -2027,7 +2021,7 @@
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>67</v>
@@ -2035,7 +2029,7 @@
     </row>
     <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="4">
         <v>10</v>
@@ -2043,7 +2037,7 @@
     </row>
     <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4">
         <v>2004</v>
@@ -2059,7 +2053,7 @@
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>68</v>
@@ -2067,7 +2061,7 @@
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>69</v>
@@ -2075,7 +2069,7 @@
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>70</v>
@@ -2083,15 +2077,15 @@
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>71</v>
@@ -2139,7 +2133,7 @@
     </row>
     <row r="29" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>80</v>
@@ -2195,7 +2189,7 @@
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="4">
         <v>4.5</v>
@@ -2203,7 +2197,7 @@
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>89</v>
@@ -2211,7 +2205,7 @@
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="4">
         <v>19</v>
@@ -2219,7 +2213,7 @@
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="4">
         <v>34</v>
@@ -2227,7 +2221,7 @@
     </row>
     <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>90</v>
@@ -2235,7 +2229,7 @@
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>91</v>
@@ -2243,15 +2237,15 @@
     </row>
     <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>15</v>
@@ -2259,7 +2253,7 @@
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>15</v>
@@ -2267,7 +2261,7 @@
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B45" s="4">
         <v>70</v>
@@ -2275,7 +2269,7 @@
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>90</v>
@@ -2283,7 +2277,7 @@
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B47" s="4">
         <v>128</v>
@@ -2291,7 +2285,7 @@
     </row>
     <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B48" s="4">
         <v>130</v>
@@ -2299,7 +2293,7 @@
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B49" s="4">
         <v>129</v>
@@ -2307,7 +2301,7 @@
     </row>
     <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B50" s="4">
         <v>100</v>
@@ -2315,7 +2309,7 @@
     </row>
     <row r="51" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B51" s="4">
         <v>101</v>
@@ -2323,7 +2317,7 @@
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>89</v>
@@ -2331,7 +2325,7 @@
     </row>
     <row r="53" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>89</v>
@@ -2339,7 +2333,7 @@
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>89</v>
@@ -2347,18 +2341,18 @@
     </row>
     <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="102" x14ac:dyDescent="0.2">
@@ -2379,7 +2373,7 @@
     </row>
     <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>94</v>
@@ -2387,7 +2381,7 @@
     </row>
     <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>15</v>
@@ -2395,10 +2389,10 @@
     </row>
     <row r="61" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2413,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89138E5-4B7A-8A4C-A60B-54B878E1BA10}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2434,31 +2428,31 @@
     </row>
     <row r="2" spans="1:2" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>3</v>
@@ -2466,7 +2460,7 @@
     </row>
     <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>15</v>
@@ -2474,23 +2468,23 @@
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>15</v>
@@ -2498,7 +2492,7 @@
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="11">
         <v>45</v>
@@ -2506,15 +2500,15 @@
     </row>
     <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>15</v>
@@ -2522,7 +2516,7 @@
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="11">
         <v>53</v>
@@ -2530,7 +2524,7 @@
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>15</v>
@@ -2538,15 +2532,15 @@
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>15</v>
@@ -2554,15 +2548,15 @@
     </row>
     <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>15</v>
@@ -2570,7 +2564,7 @@
     </row>
     <row r="19" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>15</v>
@@ -2578,7 +2572,7 @@
     </row>
     <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>15</v>
@@ -2586,7 +2580,7 @@
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>15</v>
@@ -2594,7 +2588,7 @@
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>15</v>
@@ -2602,7 +2596,7 @@
     </row>
     <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>15</v>
@@ -2610,23 +2604,23 @@
     </row>
     <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>251</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" s="11">
         <v>108</v>
@@ -2634,7 +2628,7 @@
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B27" s="11">
         <v>600</v>
@@ -2642,15 +2636,15 @@
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>15</v>
@@ -2658,7 +2652,7 @@
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>15</v>
@@ -2666,7 +2660,7 @@
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>15</v>
@@ -2674,15 +2668,15 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>15</v>
@@ -2690,23 +2684,23 @@
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>15</v>
@@ -2714,23 +2708,23 @@
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>15</v>
@@ -2738,15 +2732,15 @@
     </row>
     <row r="40" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>15</v>
@@ -2754,63 +2748,63 @@
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>15</v>
@@ -2818,7 +2812,7 @@
     </row>
     <row r="50" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>15</v>
@@ -2826,15 +2820,15 @@
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>15</v>
@@ -2842,15 +2836,15 @@
     </row>
     <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>15</v>
@@ -2858,15 +2852,15 @@
     </row>
     <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>15</v>
@@ -2874,12 +2868,12 @@
     </row>
     <row r="57" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>15</v>
@@ -2887,7 +2881,7 @@
     </row>
     <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>15</v>
@@ -2895,15 +2889,15 @@
     </row>
     <row r="60" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>15</v>
@@ -2911,15 +2905,15 @@
     </row>
     <row r="62" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>15</v>
@@ -2927,7 +2921,7 @@
     </row>
     <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>15</v>
@@ -2935,7 +2929,7 @@
     </row>
     <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B65" s="11">
         <v>1</v>
@@ -2943,15 +2937,15 @@
     </row>
     <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>15</v>
@@ -2959,15 +2953,15 @@
     </row>
     <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>15</v>
@@ -2975,15 +2969,15 @@
     </row>
     <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>15</v>
@@ -2991,7 +2985,7 @@
     </row>
     <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>15</v>
@@ -2999,7 +2993,7 @@
     </row>
     <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>15</v>
@@ -3007,7 +3001,7 @@
     </row>
     <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>15</v>
@@ -3015,7 +3009,7 @@
     </row>
     <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>15</v>
@@ -3023,15 +3017,15 @@
     </row>
     <row r="76" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>15</v>
@@ -3039,23 +3033,23 @@
     </row>
     <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>15</v>
@@ -3063,7 +3057,7 @@
     </row>
     <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>15</v>
@@ -3071,7 +3065,7 @@
     </row>
     <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>15</v>
@@ -3079,7 +3073,7 @@
     </row>
     <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>15</v>
@@ -3087,7 +3081,7 @@
     </row>
     <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>15</v>
@@ -3095,7 +3089,7 @@
     </row>
     <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>15</v>
@@ -3103,7 +3097,7 @@
     </row>
     <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B86" s="11" t="s">
         <v>15</v>
@@ -3111,23 +3105,23 @@
     </row>
     <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>15</v>
@@ -3135,7 +3129,7 @@
     </row>
     <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B90" s="11" t="s">
         <v>15</v>
@@ -3143,7 +3137,7 @@
     </row>
     <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>15</v>
@@ -3151,7 +3145,7 @@
     </row>
     <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>15</v>
@@ -3159,7 +3153,7 @@
     </row>
     <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B93" s="11" t="s">
         <v>15</v>
@@ -3167,7 +3161,7 @@
     </row>
     <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>15</v>
@@ -3175,7 +3169,7 @@
     </row>
     <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B95" s="11" t="s">
         <v>15</v>
@@ -3183,7 +3177,7 @@
     </row>
     <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B96" s="11" t="s">
         <v>15</v>
@@ -3191,7 +3185,7 @@
     </row>
     <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>15</v>
@@ -3199,7 +3193,7 @@
     </row>
     <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>15</v>
@@ -3207,7 +3201,7 @@
     </row>
     <row r="99" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>15</v>
@@ -3215,7 +3209,7 @@
     </row>
     <row r="100" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>15</v>
@@ -3223,7 +3217,7 @@
     </row>
     <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>15</v>
@@ -3231,7 +3225,7 @@
     </row>
     <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B102" s="11" t="s">
         <v>15</v>
@@ -3239,7 +3233,7 @@
     </row>
     <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>15</v>
@@ -3247,7 +3241,7 @@
     </row>
     <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>15</v>
@@ -3255,7 +3249,7 @@
     </row>
     <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B105" s="11" t="s">
         <v>15</v>
@@ -3263,127 +3257,127 @@
     </row>
     <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B121" s="11" t="s">
         <v>15</v>
@@ -3391,15 +3385,15 @@
     </row>
     <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B123" s="11" t="s">
         <v>15</v>
@@ -3407,7 +3401,7 @@
     </row>
     <row r="124" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B124" s="11" t="s">
         <v>15</v>
@@ -3415,15 +3409,15 @@
     </row>
     <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="14" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B126" s="11" t="s">
         <v>15</v>
@@ -3431,63 +3425,63 @@
     </row>
     <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B127" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="B127" s="11" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="14" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="14" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="14" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="13" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B134" s="11" t="s">
         <v>15</v>
@@ -3495,15 +3489,15 @@
     </row>
     <row r="135" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B136" s="11" t="s">
         <v>15</v>
@@ -3511,7 +3505,7 @@
     </row>
     <row r="137" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="13" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B137" s="11" t="s">
         <v>15</v>
@@ -3519,7 +3513,7 @@
     </row>
     <row r="138" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B138" s="11" t="s">
         <v>15</v>
@@ -3527,15 +3521,15 @@
     </row>
     <row r="139" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B140" s="11" t="s">
         <v>15</v>
@@ -3543,7 +3537,7 @@
     </row>
     <row r="141" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B141" s="11" t="s">
         <v>15</v>
@@ -3551,7 +3545,7 @@
     </row>
     <row r="142" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B142" s="11" t="s">
         <v>15</v>
@@ -3559,15 +3553,15 @@
     </row>
     <row r="143" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B144" s="11" t="s">
         <v>15</v>
@@ -3575,7 +3569,7 @@
     </row>
     <row r="145" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B145" s="11" t="s">
         <v>15</v>
@@ -3583,7 +3577,7 @@
     </row>
     <row r="146" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B146" s="11" t="s">
         <v>15</v>
@@ -3591,15 +3585,15 @@
     </row>
     <row r="147" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B148" s="11" t="s">
         <v>15</v>
@@ -3607,7 +3601,7 @@
     </row>
     <row r="149" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B149" s="11" t="s">
         <v>15</v>
@@ -3615,7 +3609,7 @@
     </row>
     <row r="150" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B150" s="11" t="s">
         <v>15</v>
@@ -3623,7 +3617,7 @@
     </row>
     <row r="151" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>15</v>
@@ -3631,7 +3625,7 @@
     </row>
     <row r="152" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>15</v>
@@ -3639,23 +3633,23 @@
     </row>
     <row r="153" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B155" s="11" t="s">
         <v>15</v>
@@ -3663,7 +3657,7 @@
     </row>
     <row r="156" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B156" s="11" t="s">
         <v>15</v>
@@ -3671,15 +3665,15 @@
     </row>
     <row r="157" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B158" s="11" t="s">
         <v>15</v>
@@ -3687,7 +3681,7 @@
     </row>
     <row r="159" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="13" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B159" s="11" t="s">
         <v>15</v>
@@ -3695,7 +3689,7 @@
     </row>
     <row r="160" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B160" s="11" t="s">
         <v>15</v>
@@ -3703,26 +3697,26 @@
     </row>
     <row r="161" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="128" x14ac:dyDescent="0.2">
       <c r="A163" s="13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHARMS - RAS IIQ Scenarios automation completed
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDAE67-DC76-9040-9753-852BE6540B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF14BE47-3EAF-5F42-8276-FB91D374F1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25700" yWindow="500" windowWidth="25480" windowHeight="28300" activeTab="2" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="25700" yWindow="500" windowWidth="25480" windowHeight="28300" activeTab="1" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="343">
   <si>
     <t>Question</t>
   </si>
@@ -1135,6 +1135,12 @@
   </si>
   <si>
     <t>RASTest2022$$</t>
+  </si>
+  <si>
+    <t>To determine eligibility for this study, we need to collect information about medical diagnoses.</t>
+  </si>
+  <si>
+    <t>We know that RASopathies are a group of syndromes that have a genetic basis.  In order to help us determine eligibility for the RASopathies Study, we also need to know about any genetic testing that has been completed.</t>
   </si>
 </sst>
 </file>
@@ -1565,7 +1571,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1771,9 +1777,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>341</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>38</v>
@@ -1803,9 +1809,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>271</v>
+        <v>342</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>271</v>
@@ -1896,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA38AB1-F752-BB4E-9CFB-C6D8167B319F}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2407,7 +2413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89138E5-4B7A-8A4C-A60B-54B878E1BA10}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2730,7 +2736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>152</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>153</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>155</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>258</v>
       </c>

</xml_diff>

<commit_message>
CHARMS - RAS Regression pass
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF14BE47-3EAF-5F42-8276-FB91D374F1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69A6DB3-BC37-B141-9434-618C0B3CA2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25700" yWindow="500" windowWidth="25480" windowHeight="28300" activeTab="1" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="600" yWindow="500" windowWidth="25480" windowHeight="28300" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="340">
   <si>
     <t>Question</t>
   </si>
@@ -340,12 +340,6 @@
   </si>
   <si>
     <t>16 years</t>
-  </si>
-  <si>
-    <t>Please log in. Email</t>
-  </si>
-  <si>
-    <t>Please log in. One Time Pin</t>
   </si>
   <si>
     <t xml:space="preserve">Some of this information may be difficult for you to recall completely. If you cannot remember something exactly, please give your best estimate. Feel free to consult other family members, doctors, medical records, or any other sources that may assist you.
@@ -1132,9 +1126,6 @@
   </si>
   <si>
     <t>ScreenerOneFirst</t>
-  </si>
-  <si>
-    <t>RASTest2022$$</t>
   </si>
   <si>
     <t>To determine eligibility for this study, we need to collect information about medical diagnoses.</t>
@@ -1570,13 +1561,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.33203125" customWidth="1"/>
+    <col min="1" max="1" width="98.5" customWidth="1"/>
     <col min="2" max="2" width="53" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1601,7 +1592,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1617,7 +1608,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1718,7 +1709,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1726,7 +1717,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1779,7 +1770,7 @@
     </row>
     <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>38</v>
@@ -1811,10 +1802,10 @@
     </row>
     <row r="30" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -1883,10 +1874,10 @@
     </row>
     <row r="39" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1900,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA38AB1-F752-BB4E-9CFB-C6D8167B319F}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1921,249 +1912,249 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="272" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="272" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>99</v>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>100</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
+    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>120</v>
+      </c>
+      <c r="B14" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="4">
-        <v>10</v>
+      <c r="B15" s="4">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7">
+        <v>38301</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" s="4">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="7">
-        <v>38301</v>
+        <v>100</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>68</v>
+      <c r="B19" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>15</v>
@@ -2171,90 +2162,90 @@
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>15</v>
+        <v>107</v>
+      </c>
+      <c r="B34" s="4">
+        <v>4.5</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B36" s="4">
-        <v>4.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>89</v>
+      <c r="A37" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="4">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="4">
-        <v>19</v>
+        <v>110</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>90</v>
+        <v>123</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>125</v>
+      <c r="B42" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>15</v>
+      <c r="B43" s="4">
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2262,63 +2253,63 @@
         <v>116</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B45" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>90</v>
+        <v>272</v>
+      </c>
+      <c r="B46" s="4">
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B47" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B48" s="4">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B49" s="4">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B50" s="4">
-        <v>100</v>
+      <c r="B50" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B51" s="4">
-        <v>101</v>
+      <c r="B51" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -2334,7 +2325,7 @@
         <v>278</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>89</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -2342,69 +2333,50 @@
         <v>279</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>280</v>
+        <v>92</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>281</v>
+        <v>93</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>124</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5C1CFFB7-EAA4-BF4D-9E37-A0CDDDFF3A46}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2413,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89138E5-4B7A-8A4C-A60B-54B878E1BA10}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2434,31 +2406,31 @@
     </row>
     <row r="2" spans="1:2" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>3</v>
@@ -2466,7 +2438,7 @@
     </row>
     <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>15</v>
@@ -2474,23 +2446,23 @@
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>15</v>
@@ -2498,7 +2470,7 @@
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B10" s="11">
         <v>45</v>
@@ -2506,15 +2478,15 @@
     </row>
     <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>15</v>
@@ -2522,7 +2494,7 @@
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="11">
         <v>53</v>
@@ -2530,7 +2502,7 @@
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>15</v>
@@ -2538,15 +2510,15 @@
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>15</v>
@@ -2554,15 +2526,15 @@
     </row>
     <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>15</v>
@@ -2570,7 +2542,7 @@
     </row>
     <row r="19" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>15</v>
@@ -2578,7 +2550,7 @@
     </row>
     <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>15</v>
@@ -2586,7 +2558,7 @@
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>15</v>
@@ -2594,7 +2566,7 @@
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>15</v>
@@ -2602,7 +2574,7 @@
     </row>
     <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>15</v>
@@ -2610,23 +2582,23 @@
     </row>
     <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B26" s="11">
         <v>108</v>
@@ -2634,7 +2606,7 @@
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B27" s="11">
         <v>600</v>
@@ -2642,15 +2614,15 @@
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>15</v>
@@ -2658,7 +2630,7 @@
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>15</v>
@@ -2666,7 +2638,7 @@
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>15</v>
@@ -2674,15 +2646,15 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>15</v>
@@ -2690,23 +2662,23 @@
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>15</v>
@@ -2714,23 +2686,23 @@
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>15</v>
@@ -2738,15 +2710,15 @@
     </row>
     <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>15</v>
@@ -2754,63 +2726,63 @@
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>15</v>
@@ -2818,7 +2790,7 @@
     </row>
     <row r="50" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>15</v>
@@ -2826,15 +2798,15 @@
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>15</v>
@@ -2842,15 +2814,15 @@
     </row>
     <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>15</v>
@@ -2858,15 +2830,15 @@
     </row>
     <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>15</v>
@@ -2874,12 +2846,12 @@
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>15</v>
@@ -2887,7 +2859,7 @@
     </row>
     <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>15</v>
@@ -2895,15 +2867,15 @@
     </row>
     <row r="60" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>15</v>
@@ -2911,15 +2883,15 @@
     </row>
     <row r="62" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>15</v>
@@ -2927,7 +2899,7 @@
     </row>
     <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>15</v>
@@ -2935,7 +2907,7 @@
     </row>
     <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B65" s="11">
         <v>1</v>
@@ -2943,15 +2915,15 @@
     </row>
     <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>15</v>
@@ -2959,15 +2931,15 @@
     </row>
     <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>15</v>
@@ -2975,15 +2947,15 @@
     </row>
     <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>15</v>
@@ -2991,7 +2963,7 @@
     </row>
     <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>15</v>
@@ -2999,7 +2971,7 @@
     </row>
     <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>15</v>
@@ -3007,7 +2979,7 @@
     </row>
     <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>15</v>
@@ -3015,7 +2987,7 @@
     </row>
     <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>15</v>
@@ -3023,15 +2995,15 @@
     </row>
     <row r="76" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>15</v>
@@ -3039,23 +3011,23 @@
     </row>
     <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>15</v>
@@ -3063,7 +3035,7 @@
     </row>
     <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>15</v>
@@ -3071,7 +3043,7 @@
     </row>
     <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>15</v>
@@ -3079,7 +3051,7 @@
     </row>
     <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>15</v>
@@ -3087,7 +3059,7 @@
     </row>
     <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>15</v>
@@ -3095,7 +3067,7 @@
     </row>
     <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>15</v>
@@ -3103,7 +3075,7 @@
     </row>
     <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B86" s="11" t="s">
         <v>15</v>
@@ -3111,23 +3083,23 @@
     </row>
     <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>15</v>
@@ -3135,7 +3107,7 @@
     </row>
     <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B90" s="11" t="s">
         <v>15</v>
@@ -3143,7 +3115,7 @@
     </row>
     <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>15</v>
@@ -3151,7 +3123,7 @@
     </row>
     <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>15</v>
@@ -3159,7 +3131,7 @@
     </row>
     <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B93" s="11" t="s">
         <v>15</v>
@@ -3167,7 +3139,7 @@
     </row>
     <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>15</v>
@@ -3175,7 +3147,7 @@
     </row>
     <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B95" s="11" t="s">
         <v>15</v>
@@ -3183,7 +3155,7 @@
     </row>
     <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B96" s="11" t="s">
         <v>15</v>
@@ -3191,7 +3163,7 @@
     </row>
     <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>15</v>
@@ -3199,7 +3171,7 @@
     </row>
     <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>15</v>
@@ -3207,7 +3179,7 @@
     </row>
     <row r="99" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>15</v>
@@ -3215,7 +3187,7 @@
     </row>
     <row r="100" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>15</v>
@@ -3223,7 +3195,7 @@
     </row>
     <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>15</v>
@@ -3231,7 +3203,7 @@
     </row>
     <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B102" s="11" t="s">
         <v>15</v>
@@ -3239,7 +3211,7 @@
     </row>
     <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>15</v>
@@ -3247,7 +3219,7 @@
     </row>
     <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>15</v>
@@ -3255,7 +3227,7 @@
     </row>
     <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B105" s="11" t="s">
         <v>15</v>
@@ -3263,127 +3235,127 @@
     </row>
     <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B121" s="11" t="s">
         <v>15</v>
@@ -3391,15 +3363,15 @@
     </row>
     <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B123" s="11" t="s">
         <v>15</v>
@@ -3407,7 +3379,7 @@
     </row>
     <row r="124" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B124" s="11" t="s">
         <v>15</v>
@@ -3415,15 +3387,15 @@
     </row>
     <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B126" s="11" t="s">
         <v>15</v>
@@ -3431,63 +3403,63 @@
     </row>
     <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B134" s="11" t="s">
         <v>15</v>
@@ -3495,15 +3467,15 @@
     </row>
     <row r="135" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B136" s="11" t="s">
         <v>15</v>
@@ -3511,7 +3483,7 @@
     </row>
     <row r="137" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B137" s="11" t="s">
         <v>15</v>
@@ -3519,7 +3491,7 @@
     </row>
     <row r="138" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B138" s="11" t="s">
         <v>15</v>
@@ -3527,15 +3499,15 @@
     </row>
     <row r="139" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B140" s="11" t="s">
         <v>15</v>
@@ -3543,7 +3515,7 @@
     </row>
     <row r="141" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B141" s="11" t="s">
         <v>15</v>
@@ -3551,7 +3523,7 @@
     </row>
     <row r="142" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B142" s="11" t="s">
         <v>15</v>
@@ -3559,15 +3531,15 @@
     </row>
     <row r="143" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B144" s="11" t="s">
         <v>15</v>
@@ -3575,7 +3547,7 @@
     </row>
     <row r="145" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B145" s="11" t="s">
         <v>15</v>
@@ -3583,7 +3555,7 @@
     </row>
     <row r="146" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B146" s="11" t="s">
         <v>15</v>
@@ -3591,15 +3563,15 @@
     </row>
     <row r="147" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B148" s="11" t="s">
         <v>15</v>
@@ -3607,7 +3579,7 @@
     </row>
     <row r="149" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B149" s="11" t="s">
         <v>15</v>
@@ -3615,7 +3587,7 @@
     </row>
     <row r="150" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B150" s="11" t="s">
         <v>15</v>
@@ -3623,7 +3595,7 @@
     </row>
     <row r="151" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>15</v>
@@ -3631,7 +3603,7 @@
     </row>
     <row r="152" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>15</v>
@@ -3639,23 +3611,23 @@
     </row>
     <row r="153" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B155" s="11" t="s">
         <v>15</v>
@@ -3663,7 +3635,7 @@
     </row>
     <row r="156" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B156" s="11" t="s">
         <v>15</v>
@@ -3671,15 +3643,15 @@
     </row>
     <row r="157" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B158" s="11" t="s">
         <v>15</v>
@@ -3687,7 +3659,7 @@
     </row>
     <row r="159" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B159" s="11" t="s">
         <v>15</v>
@@ -3695,7 +3667,7 @@
     </row>
     <row r="160" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B160" s="11" t="s">
         <v>15</v>
@@ -3703,26 +3675,26 @@
     </row>
     <row r="161" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="128" x14ac:dyDescent="0.2">
       <c r="A163" s="13" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHARMS RAS - Updated Questions + GitHub Actions workflow
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juarezds/Desktop/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533BEA5E-0660-494B-9E39-4956640339B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C3572-B6AE-CD4C-B935-69D2B68B78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7240" yWindow="920" windowWidth="22940" windowHeight="14300" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -1549,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,7 +1764,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
removing localEnv file to test actions
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juarezds/Desktop/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C3572-B6AE-CD4C-B935-69D2B68B78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E22997C-F0C6-D246-8E08-3E297D681B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7240" yWindow="920" windowWidth="22940" windowHeight="14300" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -1549,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>